<commit_message>
Added R11 between gnd & agnd. Swapped pinout on RJ45 connectors back.
</commit_message>
<xml_diff>
--- a/FLS ADC BOM.xlsx
+++ b/FLS ADC BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="13200" windowWidth="34840" windowHeight="10460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="142">
   <si>
     <t>ITEM</t>
   </si>
@@ -75,18 +75,9 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>C1, C3, C4, C5, C6, C7, C8</t>
-  </si>
-  <si>
-    <t>C9, C10, C11, C12, C21, C26</t>
-  </si>
-  <si>
     <t>0.1uF</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>CAP CER 0.1UF 25V Y5V 0805</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>R1, R2, R3</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>V1240W</t>
   </si>
   <si>
@@ -430,6 +418,33 @@
   </si>
   <si>
     <t>RG32P4.7KBCT-ND</t>
+  </si>
+  <si>
+    <t>R4, R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/8W 0805 SMD</t>
+  </si>
+  <si>
+    <t>Jumper</t>
+  </si>
+  <si>
+    <t>ERJ-6GEY0R00V</t>
+  </si>
+  <si>
+    <t>P0.0ACT-ND</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>C1, C3, C4, C5, C6, C7, C8, C9</t>
+  </si>
+  <si>
+    <t>C10, C11, C12, C21, C26, C27</t>
   </si>
 </sst>
 </file>
@@ -955,7 +970,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1001,6 +1016,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1088,7 +1106,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="56">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1126,6 +1144,9 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1440,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G8" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1510,13 +1531,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="E3" s="24" t="s">
         <v>14</v>
@@ -1525,19 +1546,19 @@
         <v>15</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L3" s="26"/>
       <c r="M3" s="11"/>
@@ -1548,7 +1569,7 @@
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="14"/>
@@ -1571,31 +1592,31 @@
         <v>5</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" s="24">
         <v>1206</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J5" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="L5" s="26"/>
       <c r="M5" s="11"/>
@@ -1610,31 +1631,31 @@
         <v>4</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E6" s="18">
         <v>1210</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J6" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="28" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L6" s="26"/>
       <c r="M6" s="11"/>
@@ -1649,31 +1670,31 @@
         <v>2</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" s="24">
         <v>1210</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="J7" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="L7" s="26"/>
       <c r="M7" s="11"/>
@@ -1688,31 +1709,31 @@
         <v>2</v>
       </c>
       <c r="C8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>29</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>32</v>
       </c>
       <c r="E8" s="24">
         <v>1210</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H8" s="29" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J8" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L8" s="26"/>
       <c r="M8" s="11"/>
@@ -1727,7 +1748,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D9" s="15">
         <v>100</v>
@@ -1736,22 +1757,22 @@
         <v>603</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J9" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="28" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="L9" s="26"/>
       <c r="M9" s="11"/>
@@ -1763,34 +1784,34 @@
         <v>7</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>36</v>
+        <v>133</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J10" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L10" s="26"/>
       <c r="M10" s="11"/>
@@ -1805,31 +1826,31 @@
         <v>2</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E11" s="18">
         <v>603</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J11" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L11" s="26"/>
       <c r="M11" s="11"/>
@@ -1844,7 +1865,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D12" s="15">
         <v>523</v>
@@ -1853,22 +1874,22 @@
         <v>603</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J12" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L12" s="26"/>
       <c r="M12" s="11"/>
@@ -1883,68 +1904,70 @@
         <v>1</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E13" s="18">
         <v>1206</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J13" s="27" t="s">
         <v>17</v>
       </c>
       <c r="K13" s="28" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="L13" s="26"/>
       <c r="M13" s="11"/>
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" s="22" customFormat="1">
       <c r="A14" s="15">
         <v>11</v>
       </c>
       <c r="B14" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="19" t="s">
-        <v>42</v>
+        <v>134</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18">
+        <v>805</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" t="s">
-        <v>111</v>
+        <v>136</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>135</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="2">
-        <v>22112042</v>
+        <v>95</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>110</v>
+        <v>17</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>138</v>
       </c>
       <c r="L14" s="26"/>
       <c r="M14" s="11"/>
@@ -1953,35 +1976,36 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="15">
+        <f>A14+1</f>
         <v>12</v>
       </c>
       <c r="B15" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="D15" s="15"/>
-      <c r="E15" s="18" t="s">
-        <v>55</v>
+      <c r="E15" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>69</v>
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>107</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>70</v>
+        <v>40</v>
+      </c>
+      <c r="I15" s="2">
+        <v>22112042</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>68</v>
+        <v>41</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>106</v>
       </c>
       <c r="L15" s="26"/>
       <c r="M15" s="11"/>
@@ -1990,35 +2014,36 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="15">
+        <f t="shared" ref="A16:A23" si="0">A15+1</f>
         <v>13</v>
       </c>
       <c r="B16" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="H16" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>117</v>
-      </c>
       <c r="J16" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" t="s">
-        <v>116</v>
+        <v>41</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="L16" s="26"/>
       <c r="M16" s="11"/>
@@ -2027,35 +2052,36 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="15">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B17" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="21">
-        <v>471554001</v>
+        <v>111</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" s="16" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="K17" t="s">
+        <v>112</v>
       </c>
       <c r="L17" s="26"/>
       <c r="M17" s="11"/>
@@ -2064,35 +2090,36 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="15">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B18" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="D18" s="15"/>
       <c r="E18" s="18" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>71</v>
+        <v>49</v>
+      </c>
+      <c r="I18" s="21">
+        <v>471554001</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K18" s="22" t="s">
-        <v>72</v>
+        <v>41</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="L18" s="26"/>
       <c r="M18" s="11"/>
@@ -2101,109 +2128,112 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="15">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="B19" s="17">
         <v>1</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>75</v>
+        <v>41</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="L19" s="26"/>
-      <c r="M19" s="16"/>
+      <c r="M19" s="11"/>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="15">
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="B20" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D20" s="16"/>
-      <c r="E20" s="22" t="s">
-        <v>118</v>
+      <c r="E20" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>79</v>
+        <v>41</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="L20" s="26"/>
-      <c r="M20" s="11"/>
+      <c r="M20" s="16"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="15">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="B21" s="17">
         <v>2</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D21" s="16"/>
-      <c r="E21" s="18" t="s">
-        <v>63</v>
+      <c r="E21" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>64</v>
+        <v>79</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>91</v>
+        <v>77</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>78</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="K21" s="22" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="L21" s="26"/>
       <c r="M21" s="11"/>
@@ -2212,35 +2242,36 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="15">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B22" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="18" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>88</v>
       </c>
       <c r="G22" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="J22" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" s="22" t="s">
         <v>86</v>
-      </c>
-      <c r="I22" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="J22" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>85</v>
       </c>
       <c r="L22" s="26"/>
       <c r="M22" s="11"/>
@@ -2248,44 +2279,82 @@
       <c r="O22" s="13"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
+      <c r="A23" s="15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B23" s="17">
+        <v>1</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L23" s="26"/>
+      <c r="M23" s="11"/>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
     </row>
-    <row r="24" spans="1:15">
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-    </row>
-    <row r="25" spans="1:15" s="22" customFormat="1">
-      <c r="A25" s="1"/>
-      <c r="B25" s="15">
-        <f>SUM(B5:B22)</f>
-        <v>41</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="37" spans="7:7">
-      <c r="G37" s="10"/>
+    <row r="24" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="1:15" s="22" customFormat="1">
+      <c r="A26" s="1"/>
+      <c r="B26" s="9">
+        <f>SUM(B3:B23)</f>
+        <v>43</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="38" spans="7:7">
+      <c r="G38" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2299,6 +2368,8 @@
     <hyperlink ref="K9" r:id="rId8"/>
     <hyperlink ref="I13" r:id="rId9"/>
     <hyperlink ref="K13" r:id="rId10"/>
+    <hyperlink ref="I14" r:id="rId11"/>
+    <hyperlink ref="K14" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>